<commit_message>
update CD homework3 figure
</commit_message>
<xml_diff>
--- a/Application-of-Geodetic-Techniques-to-Crustal-Deformation/homework3/InputFile/smoothing_test.xlsx
+++ b/Application-of-Geodetic-Techniques-to-Crustal-Deformation/homework3/InputFile/smoothing_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chinchia120/Documents/code-class/Application-of-Geodetic-Techniques-to-Crustal-Deformation/homework3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chinchia120/Documents/code-class/Application-of-Geodetic-Techniques-to-Crustal-Deformation/homework3/InputFile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED8B3FE-45C0-B348-AE4A-C54C1D8AA594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658A87CE-9326-B847-9ECA-1C40D497875F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29420" yWindow="-1980" windowWidth="38380" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2033,7 +2033,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>